<commit_message>
alt data fra dorte + eva
</commit_message>
<xml_diff>
--- a/data/Kopi af SPRR til esbjerg_fulversion 101221.xlsx
+++ b/data/Kopi af SPRR til esbjerg_fulversion 101221.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Documents\Code\Speciale\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81C1F29E-85D0-48AA-B5AB-480BADCED06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{81C1F29E-85D0-48AA-B5AB-480BADCED06A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="hidden" xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15600" xr2:uid="{4945AC14-70B2-4790-A402-2CEEE388F912}"/>
-    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15600" xr2:uid="{F3BEDCAF-2F4D-48AD-8D56-F91ED459115A}"/>
-    <workbookView visibility="hidden" xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15600" xr2:uid="{B1D28580-2409-4DF1-802D-4DFBB9E40CE8}"/>
+    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4945AC14-70B2-4790-A402-2CEEE388F912}"/>
+    <workbookView xWindow="2145" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{F3BEDCAF-2F4D-48AD-8D56-F91ED459115A}"/>
+    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1D28580-2409-4DF1-802D-4DFBB9E40CE8}"/>
   </bookViews>
   <sheets>
     <sheet name="analyse svar" sheetId="2" r:id="rId1"/>
@@ -529,7 +529,7 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="2"/>
   </sheetViews>
@@ -2357,53 +2357,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">CY54R7KD54KC-91199970-192712</_dlc_DocId>
+    <DLCPolicyLabelLock xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
+    <DLCPolicyLabelClientValue xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">
+      <Url>https://grundfos.sharepoint.com/sites/Pro-017826/_layouts/15/DocIdRedir.aspx?ID=CY54R7KD54KC-91199970-192712</Url>
+      <Description>CY54R7KD54KC-91199970-192712</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2674,17 +2638,53 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">CY54R7KD54KC-91199970-192712</_dlc_DocId>
-    <DLCPolicyLabelLock xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
-    <DLCPolicyLabelClientValue xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">
-      <Url>https://grundfos.sharepoint.com/sites/Pro-017826/_layouts/15/DocIdRedir.aspx?ID=CY54R7KD54KC-91199970-192712</Url>
-      <Description>CY54R7KD54KC-91199970-192712</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2697,9 +2697,12 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23B5ADC-2FED-4856-AE1D-6D8A5A36E916}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F80D695E-02F0-4FF4-A9B6-96C7E8E5A419}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="add409d8-c458-45bf-bf5f-710f0ed12ba3"/>
+    <ds:schemaRef ds:uri="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2725,12 +2728,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F80D695E-02F0-4FF4-A9B6-96C7E8E5A419}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23B5ADC-2FED-4856-AE1D-6D8A5A36E916}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="add409d8-c458-45bf-bf5f-710f0ed12ba3"/>
-    <ds:schemaRef ds:uri="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>